<commit_message>
DP - main.ipynb - finish
</commit_message>
<xml_diff>
--- a/betshemesh_muni/Intermediates/BShemesh_final.xlsx
+++ b/betshemesh_muni/Intermediates/BShemesh_final.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>moe_mosdot_coordinates</t>
+  </si>
+  <si>
+    <t>manual</t>
   </si>
 </sst>
 </file>
@@ -1185,6 +1188,18 @@
       </c>
     </row>
     <row r="31" spans="1:8">
+      <c r="A31">
+        <v>673392</v>
+      </c>
+      <c r="B31">
+        <v>623728.0756</v>
+      </c>
+      <c r="C31">
+        <v>199204.9726</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
       <c r="E31">
         <v>2</v>
       </c>
@@ -1565,6 +1580,15 @@
     <row r="46" spans="1:8">
       <c r="A46">
         <v>641639</v>
+      </c>
+      <c r="B46">
+        <v>198662</v>
+      </c>
+      <c r="C46">
+        <v>627760</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
       </c>
       <c r="E46">
         <v>3</v>

</xml_diff>